<commit_message>
fixed error in PnP file
</commit_message>
<xml_diff>
--- a/spear-dev-board/PnP file.xlsx
+++ b/spear-dev-board/PnP file.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Gerber\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Download\pcb_designs\spear-dev-board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18219D0A-76BD-4CCC-AE71-B744B7F189A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80194889-D3BD-4A6E-86DA-0B98B76CA2D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
     <t>X2</t>
   </si>
   <si>
-    <t>g</t>
+    <t>C1</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E38"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>

</xml_diff>